<commit_message>
Updated Sheet Creation and Difference Formatting
</commit_message>
<xml_diff>
--- a/Test2.xlsx
+++ b/Test2.xlsx
@@ -2,26 +2,221 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GG-Code\source\repos\Web Scraping and Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gnjg1\Python Repos\Web_Scraping_App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD76133-FB4C-48EB-B471-BF4E2FD923D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C0C0E6A-5304-477B-B7D4-3D6960ADC0D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8832" yWindow="2388" windowWidth="30960" windowHeight="12660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="02_13_2021" sheetId="2" r:id="rId1"/>
-    <sheet name="02_19_2021" sheetId="1" r:id="rId2"/>
+    <sheet name="For-Copy" sheetId="1" state="veryHidden" r:id="rId1"/>
+    <sheet name="Table of Contents" sheetId="2" r:id="rId2"/>
+    <sheet name="02_13_2021" sheetId="3" r:id="rId3"/>
+    <sheet name="02_19_2021" sheetId="4" r:id="rId4"/>
+    <sheet name="02_28_2021" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="73">
+  <si>
+    <t>CoBank</t>
+  </si>
+  <si>
+    <t>AgFirst</t>
+  </si>
+  <si>
+    <t>AgriBank</t>
+  </si>
+  <si>
+    <t>Texas FCB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name </t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Checked</t>
+  </si>
+  <si>
+    <t>Thomas Halverson</t>
+  </si>
+  <si>
+    <t>President and Chief Executive Officer</t>
+  </si>
+  <si>
+    <t>02_13_2021</t>
+  </si>
+  <si>
+    <t>TIM AMERSON</t>
+  </si>
+  <si>
+    <t>PRESIDENT AND CHIEF EXECUTIVE OFFICER</t>
+  </si>
+  <si>
+    <t>Jeffrey Swanhorst</t>
+  </si>
+  <si>
+    <t>Chief Executive Officer</t>
+  </si>
+  <si>
+    <t>AMIE PALA</t>
+  </si>
+  <si>
+    <t>CHIEF EXECUTIVE OFFICER</t>
+  </si>
+  <si>
+    <t>Deboleena Bose</t>
+  </si>
+  <si>
+    <t>Chief Human Resources Officer</t>
+  </si>
+  <si>
+    <t>CHARL BUTLER</t>
+  </si>
+  <si>
+    <t>EXECUTIVE VICE PRESIDENT AND CHIEF OPERATING OFFICER</t>
+  </si>
+  <si>
+    <t>John Grace</t>
+  </si>
+  <si>
+    <t>Chief Risk Officer</t>
+  </si>
+  <si>
+    <t>BRANDON BLAUT</t>
+  </si>
+  <si>
+    <t>CHIEF FINANCIAL OFFICER</t>
+  </si>
+  <si>
+    <t>David P. Burlage</t>
+  </si>
+  <si>
+    <t>Chief Financial Officer</t>
+  </si>
+  <si>
+    <t>ISVARA WILSON</t>
+  </si>
+  <si>
+    <t>EXECUTIVE VICE PRESIDENT AND CHIEF ADMINISTRATIVE OFFICER</t>
+  </si>
+  <si>
+    <t>Jim Jones</t>
+  </si>
+  <si>
+    <t>Chief Credit Officer</t>
+  </si>
+  <si>
+    <t>JOHN SLOAN</t>
+  </si>
+  <si>
+    <t>CHIEF CREDIT OFFICER</t>
+  </si>
+  <si>
+    <t>Timothy Curran</t>
+  </si>
+  <si>
+    <t>WILL BROWN</t>
+  </si>
+  <si>
+    <t>SENIOR VICE PRESIDENT AND CHIEF CREDIT OFFICER</t>
+  </si>
+  <si>
+    <t>Jeff Moore</t>
+  </si>
+  <si>
+    <t>NANCI TUCKER</t>
+  </si>
+  <si>
+    <t>GENERAL COUNSEL</t>
+  </si>
+  <si>
+    <t>Bill Davis</t>
+  </si>
+  <si>
+    <t>Executive Vice President, Farm Credit Banking Group</t>
+  </si>
+  <si>
+    <t>JAMIE BUMGARNER</t>
+  </si>
+  <si>
+    <t>VICE PRESIDENT AND DIRECTOR OF ASSOCIATION RELATIONSHIPS</t>
+  </si>
+  <si>
+    <t>Barbara Stille</t>
+  </si>
+  <si>
+    <t>Chief Administrative Officer and General Counsel</t>
+  </si>
+  <si>
+    <t>NISHA ROCAP</t>
+  </si>
+  <si>
+    <t>CHIEF AUDIT EXECUTIVE</t>
+  </si>
+  <si>
+    <t>Eric Itambo</t>
+  </si>
+  <si>
+    <t>Chief Banking Officer</t>
+  </si>
+  <si>
+    <t>STEPHEN “STEVE” CIAMBRONE</t>
+  </si>
+  <si>
+    <t>SENIOR VICE PRESIDENT AND CHIEF INFORMATION OFFICER</t>
+  </si>
+  <si>
+    <t>Barack Obama</t>
+  </si>
+  <si>
+    <t>Carmen Sandiego</t>
+  </si>
+  <si>
+    <t>Andrew D. Jacob</t>
+  </si>
+  <si>
+    <t>Chief Operating Officer</t>
+  </si>
+  <si>
+    <t>STEPHEN GILBERT</t>
+  </si>
+  <si>
+    <t>SENIOR VICE PRESIDENT AND CHIEF FINANCIAL OFFICER</t>
+  </si>
+  <si>
+    <t>M. Mashenka Lundberg</t>
+  </si>
+  <si>
+    <t>Chief Legal Officer and General Counsel</t>
+  </si>
+  <si>
+    <t>FRANCES GRIGGS</t>
+  </si>
+  <si>
+    <t>SENIOR VICE PRESIDENT AND GENERAL COUNSEL</t>
+  </si>
+  <si>
+    <t>Waldo</t>
+  </si>
+  <si>
+    <t>DAN LAFRENIERE</t>
+  </si>
+  <si>
+    <t>SENIOR VICE PRESIDENT AND CHIEF AUDIT EXECUTIVE</t>
+  </si>
+  <si>
+    <t>Red Herring</t>
+  </si>
   <si>
     <t>{'Waldo'}</t>
   </si>
@@ -35,190 +230,19 @@
     <t>{'Carmen Sandiego'}</t>
   </si>
   <si>
-    <t>Thomas Halverson</t>
-  </si>
-  <si>
-    <t>President and Chief Executive Officer</t>
-  </si>
-  <si>
     <t>02_19_2021</t>
   </si>
   <si>
-    <t>TIM AMERSON</t>
-  </si>
-  <si>
-    <t>PRESIDENT AND CHIEF EXECUTIVE OFFICER</t>
-  </si>
-  <si>
-    <t>Jeffrey Swanhorst</t>
-  </si>
-  <si>
-    <t>Chief Executive Officer</t>
-  </si>
-  <si>
-    <t>AMIE PALA</t>
-  </si>
-  <si>
-    <t>CHIEF EXECUTIVE OFFICER</t>
-  </si>
-  <si>
-    <t>Deboleena Bose</t>
-  </si>
-  <si>
-    <t>Chief Human Resources Officer</t>
-  </si>
-  <si>
-    <t>CHARL BUTLER</t>
-  </si>
-  <si>
-    <t>EXECUTIVE VICE PRESIDENT AND CHIEF OPERATING OFFICER</t>
-  </si>
-  <si>
-    <t>John Grace</t>
-  </si>
-  <si>
     <t>Chief Risk Officer and Chief Information Officer</t>
   </si>
   <si>
-    <t>BRANDON BLAUT</t>
-  </si>
-  <si>
-    <t>CHIEF FINANCIAL OFFICER</t>
-  </si>
-  <si>
-    <t>David P. Burlage</t>
-  </si>
-  <si>
-    <t>Chief Financial Officer</t>
-  </si>
-  <si>
-    <t>ISVARA WILSON</t>
-  </si>
-  <si>
-    <t>EXECUTIVE VICE PRESIDENT AND CHIEF ADMINISTRATIVE OFFICER</t>
-  </si>
-  <si>
-    <t>Jim Jones</t>
-  </si>
-  <si>
-    <t>Chief Credit Officer</t>
-  </si>
-  <si>
-    <t>JOHN SLOAN</t>
-  </si>
-  <si>
-    <t>CHIEF CREDIT OFFICER</t>
-  </si>
-  <si>
-    <t>Timothy Curran</t>
-  </si>
-  <si>
-    <t>Chief Risk Officer</t>
-  </si>
-  <si>
-    <t>WILL BROWN</t>
-  </si>
-  <si>
-    <t>SENIOR VICE PRESIDENT AND CHIEF CREDIT OFFICER</t>
-  </si>
-  <si>
-    <t>Jeff Moore</t>
-  </si>
-  <si>
-    <t>NANCI TUCKER</t>
-  </si>
-  <si>
-    <t>GENERAL COUNSEL</t>
-  </si>
-  <si>
-    <t>Bill Davis</t>
-  </si>
-  <si>
-    <t>Executive Vice President, Farm Credit Banking Group</t>
-  </si>
-  <si>
-    <t>JAMIE BUMGARNER</t>
-  </si>
-  <si>
-    <t>VICE PRESIDENT AND DIRECTOR OF ASSOCIATION RELATIONSHIPS</t>
-  </si>
-  <si>
-    <t>Barbara Stille</t>
-  </si>
-  <si>
-    <t>Chief Administrative Officer and General Counsel</t>
-  </si>
-  <si>
-    <t>NISHA ROCAP</t>
-  </si>
-  <si>
-    <t>CHIEF AUDIT EXECUTIVE</t>
-  </si>
-  <si>
-    <t>Eric Itambo</t>
-  </si>
-  <si>
-    <t>Chief Banking Officer</t>
-  </si>
-  <si>
-    <t>STEPHEN “STEVE” CIAMBRONE</t>
-  </si>
-  <si>
-    <t>SENIOR VICE PRESIDENT AND CHIEF INFORMATION OFFICER</t>
-  </si>
-  <si>
-    <t>Andrew D. Jacob</t>
-  </si>
-  <si>
-    <t>Chief Operating Officer</t>
-  </si>
-  <si>
-    <t>STEPHEN GILBERT</t>
-  </si>
-  <si>
-    <t>SENIOR VICE PRESIDENT AND CHIEF FINANCIAL OFFICER</t>
-  </si>
-  <si>
-    <t>M. Mashenka Lundberg</t>
-  </si>
-  <si>
-    <t>Chief Legal Officer and General Counsel</t>
-  </si>
-  <si>
-    <t>FRANCES GRIGGS</t>
-  </si>
-  <si>
-    <t>SENIOR VICE PRESIDENT AND GENERAL COUNSEL</t>
-  </si>
-  <si>
-    <t>DAN LAFRENIERE</t>
-  </si>
-  <si>
-    <t>SENIOR VICE PRESIDENT AND CHIEF AUDIT EXECUTIVE</t>
-  </si>
-  <si>
-    <t>02_13_2021</t>
-  </si>
-  <si>
-    <t>Barack Obama</t>
-  </si>
-  <si>
-    <t>Carmen Sandiego</t>
-  </si>
-  <si>
-    <t>Waldo</t>
-  </si>
-  <si>
-    <t>Red Herring</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name </t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Checked</t>
+    <t>Obvious Difference</t>
+  </si>
+  <si>
+    <t>02_28_2021</t>
+  </si>
+  <si>
+    <t>{'Obvious Difference'}</t>
   </si>
 </sst>
 </file>
@@ -242,7 +266,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -253,6 +277,11 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA7A7"/>
       </patternFill>
     </fill>
   </fills>
@@ -268,8 +297,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -575,302 +606,400 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="B3:M4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:M3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="B5:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="56.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="41.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G5" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="H5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J5" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="K5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="L5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M5" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="H6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I6" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="J6" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="K6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="M6" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G7" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="H7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J7" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="K7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="L7" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M7" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G8" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="H8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I8" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="J8" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="K8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M8" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G9" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="H9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J9" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="K9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="M9" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G10" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="H10" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="K10" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F11" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="G11" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
         <v>58</v>
       </c>
-      <c r="E12" t="s">
-        <v>54</v>
-      </c>
       <c r="F12" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="G12" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" t="s">
         <v>61</v>
       </c>
-      <c r="E13" t="s">
-        <v>56</v>
-      </c>
       <c r="F13" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="G13" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="E14" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -878,349 +1007,353 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="B3:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="56.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="41.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
+      <c r="B3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>63</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>63</v>
+        <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>64</v>
+        <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>65</v>
+        <v>6</v>
       </c>
       <c r="H4" t="s">
-        <v>63</v>
+        <v>4</v>
       </c>
       <c r="I4" t="s">
-        <v>64</v>
+        <v>5</v>
       </c>
       <c r="J4" t="s">
-        <v>65</v>
+        <v>6</v>
       </c>
       <c r="K4" t="s">
-        <v>63</v>
+        <v>4</v>
       </c>
       <c r="L4" t="s">
-        <v>64</v>
+        <v>5</v>
       </c>
       <c r="M4" t="s">
-        <v>65</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G5" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="H5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J5" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="K5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="L5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M5" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="H6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I6" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="J6" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="K6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="M6" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G7" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="H7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J7" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="K7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="L7" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M7" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G8" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="H8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I8" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="J8" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="K8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M8" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G9" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="H9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J9" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="K9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="M9" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G10" t="s">
-        <v>6</v>
+        <v>68</v>
+      </c>
+      <c r="K10" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="E11" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F11" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="G11" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F12" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="G12" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="E13" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="F13" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="G13" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1232,4 +1365,151 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="B3:M10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="K5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="K6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="K7" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="K8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L8" t="s">
+        <v>37</v>
+      </c>
+      <c r="M8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="K9" t="s">
+        <v>44</v>
+      </c>
+      <c r="L9" t="s">
+        <v>45</v>
+      </c>
+      <c r="M9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="K10" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:M3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>